<commit_message>
updated screenshot and add saliva lib
</commit_message>
<xml_diff>
--- a/lib/APGCMS/APGCMS/lib/lib_urine_20160406.xlsx
+++ b/lib/APGCMS/APGCMS/lib/lib_urine_20160406.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="1720" windowWidth="20420" windowHeight="12600" tabRatio="500"/>
+    <workbookView xWindow="27340" yWindow="160" windowWidth="25220" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="lib_urine_20160329.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="589">
   <si>
     <t>SeqIndex</t>
   </si>
@@ -1783,13 +1783,16 @@
   </si>
   <si>
     <t xml:space="preserve">2993 131840 117184 783936 50128 44168 2186 477 3414 5366 7652 7692 22840 5300 30528 80040 191616 17240 29776 4439 7963 5350 7856 27688 6297 1060 7044 17408 25960 4673024 439616 332032 27248 40752 6038 24080 1929 3324 20520 2535 9346 1360 7139 81928 12490 51008 15740 8352 1524 7167 3872 3686 1855 7184 1196 6256 6712 26800 15651 34248 7836 26648 5307 10777 2784 4080 1130 3288 24624 7363 47784 10916 43904 12153 24576 6129 9126 1633 601 1927 1972 6363 3085 2931 3834 2980 64096 175232 23800 99272 23024 53560 5887 2704 2875 1336 658 673 3678 1072 7865 612224 105632 96536 17440 32872 5361 4629 1248 1424 2555 512 6644 1155 35280 27784 122608 29368 71200 30920 7902 2999 1806 685 531 2502 2617 11536 7350 80648 59256 93216 27832 13761 3382 1029 444 410 1401 1570 7398 5694 33416 88568 374208 353600 75184 17872 4868 810 416 1274 475 2632 3188 15240 56728 76912 24056 113928 17040 9347 281 254 849 887 865 1716 1129 11981 4807 40040 256000 52736 21832 2333 531 271 1383 950 6421 3130 15490 30168 110008 26928 19168 3552 917 753 544 1652 654 17456 255360 97672 80008 16480 9847 1893 166 289 160 3922 2596 81520 35296 349824 81088 39688 5953 427 385 1131 499 5113 101336 34112 16162 5722 1965 447 206 178 1146 4448 2900 49616 5081600 1516544 601856 105200 17456 1495 270 1160 1365 3105 4847 23360 7021 3092 410 228 404 229 167 690 7238 3602 11529 18800 6740 2100 322 153 226 561 4121 930 1669 904 314 386 784 323 9951 3365 1242 393 208 2145 267520 87200 39816 8695 1790 651 288 152 639 1175 229 288 272 160 401 155648 46752 19192 5106 1122 435 32000 8840 4005 1136 232 308 208 192 258 265 194 177 278 494 351 227 297 166 336 221 </t>
+  </si>
+  <si>
+    <t>one peak only?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1830,6 +1833,17 @@
     <font>
       <sz val="10"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1996,7 +2010,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2018,6 +2032,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2457,10 +2473,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N135"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+    <sheetView tabSelected="1" topLeftCell="B65" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5312,21 +5331,23 @@
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="17">
         <v>22.46</v>
       </c>
-      <c r="F76" s="9">
+      <c r="F76" s="18">
         <v>1594.17</v>
       </c>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
       <c r="J76" t="s">
         <v>312</v>
       </c>
@@ -6690,7 +6711,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:15">
       <c r="A113">
         <v>112</v>
       </c>
@@ -6728,7 +6749,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:15">
       <c r="A114">
         <v>114</v>
       </c>
@@ -6772,7 +6793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:15">
       <c r="A115">
         <v>113</v>
       </c>
@@ -6813,7 +6834,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:15">
       <c r="A116">
         <v>115</v>
       </c>
@@ -6851,7 +6872,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:15">
       <c r="A117">
         <v>116</v>
       </c>
@@ -6889,7 +6910,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:15">
       <c r="A118">
         <v>117</v>
       </c>
@@ -6927,7 +6948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:15">
       <c r="A119">
         <v>118</v>
       </c>
@@ -6962,7 +6983,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:15">
       <c r="A120">
         <v>119</v>
       </c>
@@ -6997,7 +7018,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:15">
       <c r="A121">
         <v>120</v>
       </c>
@@ -7035,7 +7056,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:15">
       <c r="A122">
         <v>121</v>
       </c>
@@ -7073,7 +7094,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:15">
       <c r="A123">
         <v>122</v>
       </c>
@@ -7111,7 +7132,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:15">
       <c r="A124">
         <v>123</v>
       </c>
@@ -7149,7 +7170,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:15">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7187,7 +7208,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:14">
+    <row r="126" spans="1:15">
       <c r="A126">
         <v>125</v>
       </c>
@@ -7225,7 +7246,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="127" spans="1:14">
+    <row r="127" spans="1:15">
       <c r="A127">
         <v>126</v>
       </c>
@@ -7263,79 +7284,82 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:14">
-      <c r="A128">
+    <row r="128" spans="1:15" s="1" customFormat="1">
+      <c r="A128" s="1">
         <v>127</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="E128">
+      <c r="E128" s="1">
         <v>31.82</v>
       </c>
-      <c r="F128" s="9">
+      <c r="F128" s="10">
         <v>2157.1999999999998</v>
       </c>
-      <c r="G128">
+      <c r="G128" s="1">
         <v>260</v>
       </c>
-      <c r="H128">
+      <c r="H128" s="1">
         <v>218</v>
       </c>
-      <c r="J128" t="s">
+      <c r="J128" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="K128" t="s">
+      <c r="K128" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="L128" t="s">
-        <v>23</v>
-      </c>
-      <c r="M128" t="s">
+      <c r="L128" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M128" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="129" spans="1:13">
-      <c r="A129">
+      <c r="O128" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" s="1" customFormat="1">
+      <c r="A129" s="1">
         <v>128</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="E129">
+      <c r="E129" s="1">
         <v>31.82</v>
       </c>
-      <c r="F129" s="9">
+      <c r="F129" s="10">
         <v>2158</v>
       </c>
-      <c r="G129">
+      <c r="G129" s="1">
         <v>179</v>
       </c>
-      <c r="H129">
+      <c r="H129" s="1">
         <v>308</v>
       </c>
-      <c r="J129" t="s">
+      <c r="J129" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="K129" t="s">
+      <c r="K129" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="L129" t="s">
-        <v>23</v>
-      </c>
-      <c r="M129" t="s">
+      <c r="L129" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M129" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7562,11 +7586,12 @@
   <sortState ref="A2:N135">
     <sortCondition ref="F123"/>
   </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="31" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>